<commit_message>
List of continuous stations
</commit_message>
<xml_diff>
--- a/analysis_2022/data_clean/continuous_stations.xlsx
+++ b/analysis_2022/data_clean/continuous_stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9371D50F-5A9A-420B-9D90-DA22344FFACD}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBFFA13C-F54D-49DD-9403-DE402D7843DE}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11265" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>MDM</t>
   </si>
@@ -85,6 +85,48 @@
   </si>
   <si>
     <t>DSJ</t>
+  </si>
+  <si>
+    <t>BLP</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DUTCH SLOUGH AT JERSEY ISLAND</t>
+  </si>
+  <si>
+    <t>BLIND POINT</t>
+  </si>
+  <si>
+    <t>SAN JOAQUIN RIVER AT MOSSDALE BRIDGE</t>
+  </si>
+  <si>
+    <t>FALSE RIVER NEAR OAKLEY</t>
+  </si>
+  <si>
+    <t>HOLLAND CUT NEAR BETHEL ISLAND</t>
+  </si>
+  <si>
+    <t>MIDDLE RIVER NEAR HOLT</t>
+  </si>
+  <si>
+    <t>OLD RIVER AT QUIMBLY IS NEAR BETHEL IS</t>
+  </si>
+  <si>
+    <t>OLD RIVER AT FRANKS TRACT NEAR TERMINOUS</t>
+  </si>
+  <si>
+    <t>FRANK'S TRACT MID TRACT</t>
+  </si>
+  <si>
+    <t>MIDDLE RIVER AT MIDDLE RIVER</t>
+  </si>
+  <si>
+    <t>SAN JOAQUIN R MCCUNE STATION NR VERNALIS</t>
+  </si>
+  <si>
+    <t>HARVEY O BANKS PUMPING P (KA000331)</t>
   </si>
 </sst>
 </file>
@@ -452,15 +494,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA7C040-8D1D-48F7-B6B0-CC353C7A569F}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -473,8 +515,11 @@
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -487,8 +532,11 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -501,8 +549,11 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -515,8 +566,11 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -529,8 +583,11 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -543,8 +600,11 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -557,8 +617,11 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -571,8 +634,11 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -585,8 +651,11 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -599,8 +668,11 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -613,8 +685,11 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -627,17 +702,34 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>38.032451999999999</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-121.71904000000001</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pulled and plotted additional flow and velocity data; still needs updating. Added drought average to dayflow plot
</commit_message>
<xml_diff>
--- a/analysis_2022/data_clean/continuous_stations.xlsx
+++ b/analysis_2022/data_clean/continuous_stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBFFA13C-F54D-49DD-9403-DE402D7843DE}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{707BEF80-92AE-4A57-AD68-CEE3F97623E8}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>MDM</t>
   </si>
@@ -127,6 +127,24 @@
   </si>
   <si>
     <t>HARVEY O BANKS PUMPING P (KA000331)</t>
+  </si>
+  <si>
+    <t>SJG</t>
+  </si>
+  <si>
+    <t>SJC</t>
+  </si>
+  <si>
+    <t>SAN JOAQUIN RIVER NEAR BUCKLEY COVE</t>
+  </si>
+  <si>
+    <t>SAN JOAQUIN RIVER AT GARWOOD BRIDGE</t>
+  </si>
+  <si>
+    <t>VNS</t>
+  </si>
+  <si>
+    <t>SAN JOAQUIN RIVER NEAR VERNALIS</t>
   </si>
 </sst>
 </file>
@@ -136,7 +154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,16 +168,35 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -167,11 +204,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF111111"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -179,6 +231,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,7 +556,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,14 +782,56 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
+    <row r="14" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4">
+        <v>37.935000000000002</v>
+      </c>
+      <c r="C14" s="5">
+        <v>-121.32899999999999</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>37.980266</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-121.385717</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>37.676040999999998</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-121.266327</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>

</xml_diff>

<commit_message>
Added to continuous stations
</commit_message>
<xml_diff>
--- a/analysis_2022/data_clean/continuous_stations.xlsx
+++ b/analysis_2022/data_clean/continuous_stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{707BEF80-92AE-4A57-AD68-CEE3F97623E8}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA9FE21-CF05-4780-AB32-147FD798DABD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>MDM</t>
   </si>
@@ -145,6 +145,39 @@
   </si>
   <si>
     <t>SAN JOAQUIN RIVER NEAR VERNALIS</t>
+  </si>
+  <si>
+    <t>DTO</t>
+  </si>
+  <si>
+    <t>HRO</t>
+  </si>
+  <si>
+    <t>TRP</t>
+  </si>
+  <si>
+    <t>USGSCode</t>
+  </si>
+  <si>
+    <t>DELTA OUTFLOW</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>HARVEY O BANKS PUMPING PLANT</t>
+  </si>
+  <si>
+    <t>TRACY PUMPING PLANT</t>
+  </si>
+  <si>
+    <t>Dayflow</t>
+  </si>
+  <si>
+    <t>WQ, Flow, Velocity</t>
+  </si>
+  <si>
+    <t>WQ, Flow</t>
   </si>
 </sst>
 </file>
@@ -154,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +213,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -223,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -238,6 +278,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,321 +596,400 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA7C040-8D1D-48F7-B6B0-CC353C7A569F}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
+        <v>11313440</v>
+      </c>
+      <c r="C2" s="3">
         <v>38.05547</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>-121.667</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3">
+        <v>38.015819999999998</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-121.58199999999999</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3">
-        <v>38.015819999999998</v>
-      </c>
-      <c r="C3" s="3">
-        <v>-121.58199999999999</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3">
+        <v>38.003079999999997</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-121.511</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>38.003079999999997</v>
-      </c>
-      <c r="C4" s="3">
-        <v>-121.511</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
+        <v>11313434</v>
+      </c>
+      <c r="C5" s="3">
         <v>38.027119999999996</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>-121.565</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3">
+        <v>38.071249999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-121.578</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
-        <v>38.071249999999999</v>
-      </c>
-      <c r="C6" s="3">
-        <v>-121.578</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3">
+        <v>38.046419999999998</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-121.598</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3">
-        <v>38.046419999999998</v>
-      </c>
-      <c r="C7" s="3">
-        <v>-121.598</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
+        <v>11312676</v>
+      </c>
+      <c r="C8" s="3">
         <v>37.942999999999998</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>-121.53400000000001</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3">
         <v>37.678899999999999</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>-121.265</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="3">
         <v>37.801900000000003</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>-121.6203</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3">
         <v>37.786000000000001</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>-121.306</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
+        <v>11313433</v>
+      </c>
+      <c r="C12" s="3">
         <v>38.01361</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>-121.66670000000001</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3">
+        <v>38.032451999999999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-121.71904000000001</v>
+      </c>
+      <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3">
-        <v>38.032451999999999</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-121.71904000000001</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="2">
+        <v>11304810</v>
+      </c>
+      <c r="C14" s="4">
         <v>37.935000000000002</v>
       </c>
-      <c r="C14" s="5">
+      <c r="D14" s="5">
         <v>-121.32899999999999</v>
       </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
       <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2"/>
+      <c r="C15">
         <v>37.980266</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>-121.385717</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
+        <v>11303500</v>
+      </c>
+      <c r="C16">
         <v>37.676040999999998</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>-121.266327</v>
       </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
       <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2">
+        <v>11303500</v>
+      </c>
+      <c r="C17">
+        <v>38.058999999999997</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-122.02500000000001</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18">
+        <v>37.798000000000002</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-121.623</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-121.58499999999999</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Saving continuous code before making changes to plots - compare MI instead.
</commit_message>
<xml_diff>
--- a/analysis_2022/data_clean/continuous_stations.xlsx
+++ b/analysis_2022/data_clean/continuous_stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA9FE21-CF05-4780-AB32-147FD798DABD}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D01C0F9-F429-434B-82B6-5752294B7F7F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>MDM</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>WQ, Flow</t>
+  </si>
+  <si>
+    <t>FCT</t>
+  </si>
+  <si>
+    <t>LIS</t>
+  </si>
+  <si>
+    <t>FISHERMANS CUT</t>
+  </si>
+  <si>
+    <t>YOLO BYPASS AT LISBON</t>
   </si>
 </sst>
 </file>
@@ -596,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA7C040-8D1D-48F7-B6B0-CC353C7A569F}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,236 +754,266 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2">
-        <v>11312676</v>
-      </c>
+      <c r="A8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="3">
-        <v>37.942999999999998</v>
+        <v>38.067822</v>
       </c>
       <c r="D8" s="3">
-        <v>-121.53400000000001</v>
+        <v>-121.648838</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
+      <c r="A9" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3">
-        <v>37.678899999999999</v>
+        <v>38.474781</v>
       </c>
       <c r="D9" s="3">
-        <v>-121.265</v>
+        <v>-121.58822600000001</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>11312676</v>
+      </c>
       <c r="C10" s="3">
-        <v>37.801900000000003</v>
+        <v>37.942999999999998</v>
       </c>
       <c r="D10" s="3">
-        <v>-121.6203</v>
+        <v>-121.53400000000001</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3">
-        <v>37.786000000000001</v>
+        <v>37.678899999999999</v>
       </c>
       <c r="D11" s="3">
-        <v>-121.306</v>
+        <v>-121.265</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2">
-        <v>11313433</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="3">
-        <v>38.01361</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-121.66670000000001</v>
+        <v>37.801900000000003</v>
+      </c>
+      <c r="D12" s="3">
+        <v>-121.6203</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>17</v>
+      <c r="A13" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3">
-        <v>38.032451999999999</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-121.71904000000001</v>
+        <v>37.786000000000001</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-121.306</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
-        <v>11304810</v>
-      </c>
-      <c r="C14" s="4">
-        <v>37.935000000000002</v>
-      </c>
-      <c r="D14" s="5">
-        <v>-121.32899999999999</v>
+        <v>11313433</v>
+      </c>
+      <c r="C14" s="3">
+        <v>38.01361</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-121.66670000000001</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15">
-        <v>37.980266</v>
+      <c r="C15" s="3">
+        <v>38.032451999999999</v>
       </c>
       <c r="D15" s="1">
-        <v>-121.385717</v>
+        <v>-121.71904000000001</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2">
+        <v>11304810</v>
+      </c>
+      <c r="C16" s="4">
+        <v>37.935000000000002</v>
+      </c>
+      <c r="D16" s="5">
+        <v>-121.32899999999999</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17">
+        <v>37.980266</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-121.385717</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="2">
-        <v>11303500</v>
-      </c>
-      <c r="C16">
-        <v>37.676040999999998</v>
-      </c>
-      <c r="D16" s="1">
-        <v>-121.266327</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="2">
-        <v>11303500</v>
-      </c>
-      <c r="C17">
-        <v>38.058999999999997</v>
-      </c>
-      <c r="D17" s="1">
-        <v>-122.02500000000001</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B18" s="2">
+        <v>11303500</v>
+      </c>
       <c r="C18">
-        <v>37.798000000000002</v>
+        <v>37.676040999999998</v>
       </c>
       <c r="D18" s="1">
-        <v>-121.623</v>
+        <v>-121.266327</v>
       </c>
       <c r="E18" t="s">
         <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="B19" s="2">
+        <v>11303500</v>
+      </c>
       <c r="C19">
-        <v>37.799999999999997</v>
+        <v>38.058999999999997</v>
       </c>
       <c r="D19" s="1">
-        <v>-121.58499999999999</v>
+        <v>-122.02500000000001</v>
       </c>
       <c r="E19" t="s">
         <v>45</v>
       </c>
       <c r="F19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20">
+        <v>37.798000000000002</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-121.623</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-121.58499999999999</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
@@ -990,6 +1032,12 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated continuous station with LIB
</commit_message>
<xml_diff>
--- a/analysis_2022/data_clean/continuous_stations.xlsx
+++ b/analysis_2022/data_clean/continuous_stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C57CD2BB-555F-4AD0-99DE-F7EF9FBDCAF7}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{72A71DD6-4F30-4CBC-B54E-21B51AEDE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71A3EC31-C2D4-45D1-AAE2-F7DD472D93E3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
+    <workbookView xWindow="31020" yWindow="1755" windowWidth="21600" windowHeight="11040" xr2:uid="{E43C89DB-75C2-428F-88E0-51B77BDDABCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>MDM</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>FISHERMANS CUT</t>
-  </si>
-  <si>
-    <t>YOLO BYPASS AT LISBON</t>
   </si>
   <si>
     <t>LIB</t>
@@ -611,7 +608,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C9" sqref="C9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +770,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3">
@@ -784,9 +781,6 @@
       </c>
       <c r="E9" t="s">
         <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>